<commit_message>
Analiza programów - całka + mnożenie macierzy
Dodane tez wykresy zużycia, czasy wykonań i zebrane temperatury
urządzeń. Dodany opis algorytmów
</commit_message>
<xml_diff>
--- a/Benchmarks-results/całka wykresy/całka - zmienny GWS 1 GPU.xlsx
+++ b/Benchmarks-results/całka wykresy/całka - zmienny GWS 1 GPU.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>GWS</t>
   </si>
@@ -95,6 +95,12 @@
   <si>
     <t>GWS 262 144</t>
   </si>
+  <si>
+    <t>całkowite zużycie energii: [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWS </t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +108,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -159,16 +165,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1834,11 +1843,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="99300096"/>
-        <c:axId val="99302784"/>
+        <c:axId val="58244480"/>
+        <c:axId val="58250368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99300096"/>
+        <c:axId val="58244480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1864,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99302784"/>
+        <c:crossAx val="58250368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1863,7 +1872,7 @@
         <c:tickLblSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99302784"/>
+        <c:axId val="58250368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1880,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99300096"/>
+        <c:crossAx val="58244480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1884,7 +1893,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2010,25 +2019,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="151253760"/>
-        <c:axId val="151255680"/>
+        <c:axId val="58256384"/>
+        <c:axId val="58258176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="151253760"/>
+        <c:axId val="58256384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151255680"/>
+        <c:crossAx val="58258176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151255680"/>
+        <c:axId val="58258176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,7 +2045,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151253760"/>
+        <c:crossAx val="58256384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2049,7 +2058,172 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>całkowite zużycie energii: [W]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$B$36:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>536870912</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>268435456</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>262144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$C$36:$C$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>11820</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1889</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1321</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1221</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1213</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="60182912"/>
+        <c:axId val="60184448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="60182912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60184448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="60184448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60182912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2059,16 +2233,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2089,16 +2263,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1781175</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2112,6 +2286,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2407,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:CZ135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5582,9 +5786,6 @@
       </c>
     </row>
     <row r="23" spans="3:40">
-      <c r="C23">
-        <v>536870912</v>
-      </c>
       <c r="M23" s="2">
         <v>0.63260416666666663</v>
       </c>
@@ -5641,9 +5842,6 @@
       </c>
     </row>
     <row r="24" spans="3:40">
-      <c r="C24">
-        <v>268435456</v>
-      </c>
       <c r="M24" s="2">
         <v>0.63261574074074078</v>
       </c>
@@ -5700,9 +5898,6 @@
       </c>
     </row>
     <row r="25" spans="3:40">
-      <c r="C25">
-        <v>134217728</v>
-      </c>
       <c r="M25" s="2">
         <v>0.63262731481481482</v>
       </c>
@@ -5759,9 +5954,6 @@
       </c>
     </row>
     <row r="26" spans="3:40">
-      <c r="C26">
-        <v>67108864</v>
-      </c>
       <c r="M26" s="2">
         <v>0.63263888888888886</v>
       </c>
@@ -5818,9 +6010,6 @@
       </c>
     </row>
     <row r="27" spans="3:40">
-      <c r="C27">
-        <v>33554432</v>
-      </c>
       <c r="M27" s="2">
         <v>0.6326504629629629</v>
       </c>
@@ -5877,9 +6066,6 @@
       </c>
     </row>
     <row r="28" spans="3:40">
-      <c r="C28">
-        <v>16777216</v>
-      </c>
       <c r="M28" s="2">
         <v>0.63266203703703705</v>
       </c>
@@ -5936,9 +6122,6 @@
       </c>
     </row>
     <row r="29" spans="3:40">
-      <c r="C29">
-        <v>8388608</v>
-      </c>
       <c r="M29" s="2">
         <v>0.63267361111111109</v>
       </c>
@@ -5995,9 +6178,6 @@
       </c>
     </row>
     <row r="30" spans="3:40">
-      <c r="C30">
-        <v>4194304</v>
-      </c>
       <c r="M30" s="2">
         <v>0.63268518518518524</v>
       </c>
@@ -6054,9 +6234,6 @@
       </c>
     </row>
     <row r="31" spans="3:40">
-      <c r="C31">
-        <v>2097152</v>
-      </c>
       <c r="M31" s="2">
         <v>0.63269675925925928</v>
       </c>
@@ -6113,9 +6290,6 @@
       </c>
     </row>
     <row r="32" spans="3:40">
-      <c r="C32">
-        <v>1048576</v>
-      </c>
       <c r="M32" s="2">
         <v>0.63270833333333332</v>
       </c>
@@ -6171,10 +6345,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="33" spans="3:33">
-      <c r="C33">
-        <v>524288</v>
-      </c>
+    <row r="33" spans="2:33">
       <c r="M33" s="2">
         <v>0.63271990740740736</v>
       </c>
@@ -6230,10 +6401,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="34" spans="3:33">
-      <c r="C34">
-        <v>262144</v>
-      </c>
+    <row r="34" spans="2:33">
       <c r="M34" s="2">
         <v>0.63273148148148151</v>
       </c>
@@ -6289,7 +6457,13 @@
         <v>928</v>
       </c>
     </row>
-    <row r="35" spans="3:33">
+    <row r="35" spans="2:33">
+      <c r="B35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="M35" s="2">
         <v>0.63274305555555554</v>
       </c>
@@ -6345,7 +6519,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="36" spans="3:33">
+    <row r="36" spans="2:33">
+      <c r="B36" s="5">
+        <v>536870912</v>
+      </c>
+      <c r="C36" s="1">
+        <f>SUM(O5:O135)</f>
+        <v>11820</v>
+      </c>
       <c r="M36" s="2">
         <v>0.63275462962962969</v>
       </c>
@@ -6401,7 +6582,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="37" spans="3:33">
+    <row r="37" spans="2:33">
+      <c r="B37" s="1">
+        <v>268435456</v>
+      </c>
+      <c r="C37" s="1">
+        <f>SUM(W5:W70)</f>
+        <v>6148</v>
+      </c>
       <c r="M37" s="2">
         <v>0.63276620370370373</v>
       </c>
@@ -6457,7 +6645,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="38" spans="3:33">
+    <row r="38" spans="2:33">
+      <c r="B38" s="1">
+        <v>134217728</v>
+      </c>
+      <c r="C38" s="1">
+        <f>SUM(AD5:AD37)</f>
+        <v>3254</v>
+      </c>
       <c r="M38" s="2">
         <v>0.63277777777777777</v>
       </c>
@@ -6495,7 +6690,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="39" spans="3:33">
+    <row r="39" spans="2:33">
+      <c r="B39" s="1">
+        <v>67108864</v>
+      </c>
+      <c r="C39" s="1">
+        <f>SUM(AK5:AK21)</f>
+        <v>1889</v>
+      </c>
       <c r="M39" s="2">
         <v>0.63278935185185181</v>
       </c>
@@ -6533,7 +6735,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="40" spans="3:33">
+    <row r="40" spans="2:33">
+      <c r="B40" s="1">
+        <v>33554432</v>
+      </c>
+      <c r="C40" s="1">
+        <f>SUM(AR5:AR15)</f>
+        <v>1346</v>
+      </c>
       <c r="M40" s="2">
         <v>0.63280092592592596</v>
       </c>
@@ -6571,7 +6780,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="41" spans="3:33">
+    <row r="41" spans="2:33">
+      <c r="B41" s="1">
+        <v>16777216</v>
+      </c>
+      <c r="C41" s="1">
+        <f>SUM(AZ5:AZ15)</f>
+        <v>1321</v>
+      </c>
       <c r="M41" s="2">
         <v>0.6328125</v>
       </c>
@@ -6609,7 +6825,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="42" spans="3:33">
+    <row r="42" spans="2:33">
+      <c r="B42" s="1">
+        <v>8388608</v>
+      </c>
+      <c r="C42" s="1">
+        <f>SUM(BH5:BH15)</f>
+        <v>1221</v>
+      </c>
       <c r="M42" s="2">
         <v>0.63282407407407404</v>
       </c>
@@ -6647,7 +6870,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="43" spans="3:33">
+    <row r="43" spans="2:33">
+      <c r="B43" s="1">
+        <v>4194304</v>
+      </c>
+      <c r="C43" s="1">
+        <f>SUM(BO5:BO15)</f>
+        <v>1213</v>
+      </c>
       <c r="M43" s="2">
         <v>0.63283564814814819</v>
       </c>
@@ -6685,7 +6915,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="44" spans="3:33">
+    <row r="44" spans="2:33">
+      <c r="B44" s="1">
+        <v>2097152</v>
+      </c>
+      <c r="C44" s="1">
+        <f>SUM(BV5:BV15)</f>
+        <v>1220</v>
+      </c>
       <c r="M44" s="2">
         <v>0.63284722222222223</v>
       </c>
@@ -6723,7 +6960,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="45" spans="3:33">
+    <row r="45" spans="2:33">
+      <c r="B45" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="C45" s="1">
+        <f>SUM(CE5:CE15)</f>
+        <v>1214</v>
+      </c>
       <c r="M45" s="2">
         <v>0.63285879629629627</v>
       </c>
@@ -6761,7 +7005,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="46" spans="3:33">
+    <row r="46" spans="2:33">
+      <c r="B46" s="1">
+        <v>524288</v>
+      </c>
+      <c r="C46" s="1">
+        <f>SUM(CN5:CN15)</f>
+        <v>1197</v>
+      </c>
       <c r="M46" s="2">
         <v>0.63287037037037031</v>
       </c>
@@ -6799,7 +7050,14 @@
         <v>928</v>
       </c>
     </row>
-    <row r="47" spans="3:33">
+    <row r="47" spans="2:33">
+      <c r="B47" s="1">
+        <v>262144</v>
+      </c>
+      <c r="C47" s="1">
+        <f>SUM(CW5:CW15)</f>
+        <v>1196</v>
+      </c>
       <c r="M47" s="2">
         <v>0.63288194444444446</v>
       </c>
@@ -6837,7 +7095,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="48" spans="3:33">
+    <row r="48" spans="2:33">
       <c r="M48" s="2">
         <v>0.63289351851851849</v>
       </c>

</xml_diff>